<commit_message>
added version to web.client assembly
</commit_message>
<xml_diff>
--- a/IkeaDocuScanV3/Documentation/InitialEndpointPermissions.xlsx
+++ b/IkeaDocuScanV3/Documentation/InitialEndpointPermissions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markr\source\repos\markRegenasst2b\IkeaDocuScan-V3\IkeaDocuScanV3\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9861DA51-88FB-4333-9909-384962F046DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C250902C-D808-4E9A-995C-57EC1124233E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{FCF8222F-3162-4C12-95FA-DB6B3F5D3B63}"/>
   </bookViews>
@@ -485,7 +485,7 @@
     <t>page missing</t>
   </si>
   <si>
-    <t>Midleware only</t>
+    <t>Midleware only for authorization</t>
   </si>
 </sst>
 </file>
@@ -630,8 +630,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D48FBC27-5723-45C8-8F7E-741F5167526D}" name="Table1" displayName="Table1" ref="A1:H118" totalsRowShown="0">
-  <autoFilter ref="A1:H118" xr:uid="{D48FBC27-5723-45C8-8F7E-741F5167526D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D48FBC27-5723-45C8-8F7E-741F5167526D}" name="Table1" displayName="Table1" ref="A1:H119" totalsRowShown="0">
+  <autoFilter ref="A1:H119" xr:uid="{D48FBC27-5723-45C8-8F7E-741F5167526D}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{E1798AA7-00B5-471D-B3B3-E3432C67E747}" name="Section"/>
     <tableColumn id="2" xr3:uid="{2A5A892E-3727-45CE-A447-CDD945476583}" name="Function"/>
@@ -965,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41ADE2EB-45D3-4E93-B349-FE5CB3F4036B}">
   <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:XFD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>